<commit_message>
Added new IMPLICIT and EXPLICIT keywords
</commit_message>
<xml_diff>
--- a/src/main/resources/TestWorkbook.xlsx
+++ b/src/main/resources/TestWorkbook.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t xml:space="preserve">Test Case</t>
   </si>
@@ -112,6 +112,12 @@
     <t>GOTOURL</t>
   </si>
   <si>
+    <t>IMPLICIT</t>
+  </si>
+  <si>
+    <t>medium_wait</t>
+  </si>
+  <si>
     <t>usernameTextField</t>
   </si>
   <si>
@@ -131,6 +137,9 @@
   </si>
   <si>
     <t>sideMenuButton</t>
+  </si>
+  <si>
+    <t>short_wait</t>
   </si>
   <si>
     <t>logoutButton</t>
@@ -205,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -220,14 +229,7 @@
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="1" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -742,13 +744,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" style="1" width="23.57421875"/>
-    <col customWidth="1" min="2" max="2" style="1" width="25.140625"/>
-    <col customWidth="1" min="3" max="3" style="1" width="23.8515625"/>
-    <col customWidth="1" min="4" max="4" style="1" width="19.28125"/>
-    <col customWidth="1" min="5" max="5" style="1" width="14.8515625"/>
-    <col min="6" max="6" style="1" width="9.140625"/>
-    <col min="7" max="16384" style="1" width="9.140625"/>
+    <col bestFit="1" customWidth="1" min="1" max="1" style="1" width="23.57421875"/>
+    <col bestFit="1" customWidth="1" min="2" max="2" style="1" width="25.140625"/>
+    <col bestFit="1" customWidth="1" min="3" max="3" style="1" width="23.8515625"/>
+    <col bestFit="1" customWidth="1" min="4" max="4" style="1" width="19.28125"/>
+    <col bestFit="1" customWidth="1" min="5" max="5" style="1" width="14.8515625"/>
+    <col bestFit="1" min="6" max="16384" style="1" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" ht="15">
@@ -776,10 +777,10 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
-      <c r="F2" s="6"/>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" s="3" customFormat="1" ht="15">
-      <c r="A3" s="7"/>
+      <c r="A3" s="5"/>
       <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
@@ -788,10 +789,10 @@
       <c r="E3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="6"/>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" s="3" customFormat="1" ht="15">
-      <c r="A4" s="7"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
@@ -804,10 +805,10 @@
       <c r="E4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="6"/>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" s="3" customFormat="1" ht="15">
-      <c r="A5" s="7"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
@@ -820,10 +821,10 @@
       <c r="E5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="6"/>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" s="3" customFormat="1" ht="15">
-      <c r="A6" s="7"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="5" t="s">
         <v>13</v>
       </c>
@@ -834,10 +835,10 @@
         <v>10</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="F6" s="6"/>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" ht="15">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="1"/>
@@ -859,7 +860,7 @@
       <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="9"/>
+      <c r="E10" s="1"/>
     </row>
     <row r="11" ht="15">
       <c r="B11" s="1" t="s">
@@ -886,15 +887,14 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" style="10" width="27.7109375"/>
-    <col customWidth="1" min="2" max="2" style="10" width="24.140625"/>
-    <col customWidth="1" min="3" max="3" style="10" width="25.57421875"/>
-    <col customWidth="1" min="4" max="4" style="10" width="15.00390625"/>
-    <col customWidth="1" min="5" max="5" style="10" width="15.28125"/>
-    <col min="6" max="6" style="10" width="9.140625"/>
-    <col min="7" max="16384" style="10" width="9.140625"/>
+    <col bestFit="1" customWidth="1" min="1" max="1" style="7" width="27.7109375"/>
+    <col bestFit="1" customWidth="1" min="2" max="2" style="7" width="24.140625"/>
+    <col bestFit="1" customWidth="1" min="3" max="3" style="7" width="25.57421875"/>
+    <col bestFit="1" customWidth="1" min="4" max="4" style="7" width="15.00390625"/>
+    <col customWidth="1" min="5" max="5" style="7" width="19.00390625"/>
+    <col bestFit="1" min="6" max="16384" style="7" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" ht="15">
@@ -919,85 +919,87 @@
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
       <c r="F2" s="3"/>
     </row>
     <row r="3" ht="15">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="3"/>
     </row>
     <row r="4" ht="15">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" ht="15">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="C5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" ht="15">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7" t="s">
+      <c r="E5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" ht="15">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="C6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" ht="15">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7" t="s">
+      <c r="E6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" ht="15">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="7" t="s">
+      <c r="C7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" ht="15">
-      <c r="A7" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" ht="15">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="A8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1006,27 +1008,27 @@
     <row r="9" ht="15">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" ht="15">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" ht="15">
@@ -1035,7 +1037,7 @@
         <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>10</v>
@@ -1046,12 +1048,26 @@
     <row r="12" ht="15">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
+    </row>
+    <row r="13" ht="15">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
Added extra keyword tests
</commit_message>
<xml_diff>
--- a/src/main/resources/TestWorkbook.xlsx
+++ b/src/main/resources/TestWorkbook.xlsx
@@ -3,10 +3,10 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Add Item to Cart" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Add to Cart" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Logout" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t xml:space="preserve">Test Case</t>
   </si>
@@ -64,76 +64,88 @@
     <t xml:space="preserve">Login to application</t>
   </si>
   <si>
-    <t xml:space="preserve">GO TO APPLICATION</t>
+    <t>GOTOURL</t>
   </si>
   <si>
     <t>login-url</t>
   </si>
   <si>
+    <t>IMPLICIT</t>
+  </si>
+  <si>
+    <t>medium_wait</t>
+  </si>
+  <si>
+    <t>ASSERT_DISPLAYED</t>
+  </si>
+  <si>
+    <t>logoImg</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
     <t>SETTEXT</t>
   </si>
   <si>
-    <t>user-name</t>
+    <t>usernameTextField</t>
   </si>
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
+    <t>standard_user</t>
+  </si>
+  <si>
+    <t>passwordTextField</t>
+  </si>
+  <si>
+    <t>secret_sauce</t>
   </si>
   <si>
     <t>CLICK</t>
   </si>
   <si>
-    <t>login-button</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add item to card</t>
+    <t>loginButton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add item</t>
+  </si>
+  <si>
+    <t>CLICK_BY_INDEX</t>
+  </si>
+  <si>
+    <t>inventoryList</t>
+  </si>
+  <si>
+    <t>inventoryItemIndex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check checkout content</t>
+  </si>
+  <si>
+    <t>shoppingCartButton</t>
+  </si>
+  <si>
+    <t>classname</t>
+  </si>
+  <si>
+    <t>ASSERT_SIZE</t>
+  </si>
+  <si>
+    <t>shoppingCartList</t>
+  </si>
+  <si>
+    <t>shoppingCartSize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logout from application</t>
   </si>
   <si>
     <t>MAXIMIZE</t>
   </si>
   <si>
     <t>EXPLICIT</t>
-  </si>
-  <si>
-    <t>short</t>
-  </si>
-  <si>
-    <t>SELECTBYINDEX</t>
-  </si>
-  <si>
-    <t>ASSERT</t>
-  </si>
-  <si>
-    <t>GOTOURL</t>
-  </si>
-  <si>
-    <t>IMPLICIT</t>
-  </si>
-  <si>
-    <t>medium_wait</t>
-  </si>
-  <si>
-    <t>usernameTextField</t>
-  </si>
-  <si>
-    <t>standard_user</t>
-  </si>
-  <si>
-    <t>passwordTextField</t>
-  </si>
-  <si>
-    <t>secret_sauce</t>
-  </si>
-  <si>
-    <t>loginButton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Logout from application</t>
   </si>
   <si>
     <t>sideMenuButton</t>
@@ -155,11 +167,6 @@
       <color theme="1"/>
       <sz val="11.000000"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Liberation Sans"/>
-      <color theme="1"/>
-      <sz val="12.000000"/>
     </font>
     <font>
       <name val="Liberation Sans"/>
@@ -177,6 +184,11 @@
     <font>
       <name val="Liberation Sans"/>
       <b/>
+      <color theme="1"/>
+      <sz val="12.000000"/>
+    </font>
+    <font>
+      <name val="Liberation Sans"/>
       <color theme="1"/>
       <sz val="12.000000"/>
     </font>
@@ -216,21 +228,21 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf fontId="1" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="3" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="4" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -744,133 +756,236 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" min="1" max="1" style="1" width="23.57421875"/>
-    <col bestFit="1" customWidth="1" min="2" max="2" style="1" width="25.140625"/>
-    <col bestFit="1" customWidth="1" min="3" max="3" style="1" width="23.8515625"/>
-    <col bestFit="1" customWidth="1" min="4" max="4" style="1" width="19.28125"/>
-    <col bestFit="1" customWidth="1" min="5" max="5" style="1" width="14.8515625"/>
-    <col bestFit="1" min="6" max="16384" style="1" width="9.140625"/>
+    <col customWidth="1" min="1" max="1" width="33.421875"/>
+    <col customWidth="1" min="2" max="2" width="26.00390625"/>
+    <col customWidth="1" min="3" max="3" width="23.7109375"/>
+    <col customWidth="1" min="4" max="4" width="15.8515625"/>
+    <col customWidth="1" min="5" max="5" width="22.00390625"/>
   </cols>
   <sheetData>
     <row r="1" ht="15">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" s="3" customFormat="1" ht="15">
-      <c r="A2" s="4" t="s">
+    <row r="2" ht="15">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" s="3" customFormat="1" ht="15">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" ht="15">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" s="3" customFormat="1" ht="15">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5" t="s">
+    </row>
+    <row r="4" ht="15">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="5" t="s">
+    </row>
+    <row r="5" ht="15">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" s="3" customFormat="1" ht="15">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" ht="15">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" ht="15">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" ht="15">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" ht="15">
+      <c r="A9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" ht="15">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" s="3" customFormat="1" ht="15">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" ht="15">
-      <c r="A7" s="6" t="s">
+      <c r="E10" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" ht="15">
+      <c r="A11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" ht="15">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" ht="15">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" ht="15">
+      <c r="A14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" ht="15">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" ht="15">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" ht="15">
-      <c r="B8" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" ht="15">
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" ht="15">
-      <c r="B10" s="1" t="s">
+      <c r="E16" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" ht="15">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" ht="15">
-      <c r="B11" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" ht="15">
-      <c r="B12" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="C17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" ht="15">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -889,185 +1004,197 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" min="1" max="1" style="7" width="27.7109375"/>
-    <col bestFit="1" customWidth="1" min="2" max="2" style="7" width="24.140625"/>
-    <col bestFit="1" customWidth="1" min="3" max="3" style="7" width="25.57421875"/>
-    <col bestFit="1" customWidth="1" min="4" max="4" style="7" width="15.00390625"/>
-    <col customWidth="1" min="5" max="5" style="7" width="19.00390625"/>
-    <col bestFit="1" min="6" max="16384" style="7" width="9.140625"/>
+    <col bestFit="1" customWidth="1" min="1" max="1" style="6" width="27.7109375"/>
+    <col bestFit="1" customWidth="1" min="2" max="2" style="6" width="26.28125"/>
+    <col bestFit="1" customWidth="1" min="3" max="3" style="6" width="25.57421875"/>
+    <col bestFit="1" customWidth="1" min="4" max="4" style="6" width="15.00390625"/>
+    <col bestFit="1" customWidth="1" min="5" max="5" style="6" width="19.00390625"/>
+    <col bestFit="1" min="6" max="16384" style="6" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" ht="15">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" ht="15">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" ht="15">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" ht="15">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="3"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" ht="15">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" ht="15">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="3"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" ht="15">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="7"/>
     </row>
     <row r="8" ht="15">
-      <c r="A8" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" ht="15">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="A9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
     </row>
     <row r="10" ht="15">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="1"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" ht="15">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="5"/>
     </row>
     <row r="12" ht="15">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
     </row>
     <row r="13" ht="15">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" ht="15">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
Added new screenshot keyword
</commit_message>
<xml_diff>
--- a/src/main/resources/TestWorkbook.xlsx
+++ b/src/main/resources/TestWorkbook.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t xml:space="preserve">Test Case</t>
   </si>
@@ -137,6 +137,12 @@
   </si>
   <si>
     <t>shoppingCartSize</t>
+  </si>
+  <si>
+    <t>SCREENSHOT</t>
+  </si>
+  <si>
+    <t>checkoutScreenShotFile</t>
   </si>
   <si>
     <t xml:space="preserve">Logout from application</t>
@@ -756,11 +762,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="33.421875"/>
-    <col customWidth="1" min="2" max="2" width="26.00390625"/>
-    <col customWidth="1" min="3" max="3" width="23.7109375"/>
-    <col customWidth="1" min="4" max="4" width="15.8515625"/>
-    <col customWidth="1" min="5" max="5" width="22.00390625"/>
+    <col bestFit="1" customWidth="1" min="1" max="1" width="33.421875"/>
+    <col bestFit="1" customWidth="1" min="2" max="2" width="26.00390625"/>
+    <col bestFit="1" customWidth="1" min="3" max="3" width="23.7109375"/>
+    <col bestFit="1" customWidth="1" min="4" max="4" width="15.8515625"/>
+    <col customWidth="1" min="5" max="5" width="26.28125"/>
   </cols>
   <sheetData>
     <row r="1" ht="15">
@@ -929,19 +935,21 @@
       </c>
     </row>
     <row r="14" ht="15">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="E14" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="15" ht="15">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="A15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -949,30 +957,26 @@
     <row r="16" ht="15">
       <c r="A16" s="5"/>
       <c r="B16" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" ht="15">
       <c r="A17" s="5"/>
       <c r="B17" s="5" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="5"/>
+      <c r="E17" s="5" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="18" ht="15">
       <c r="A18" s="5"/>
@@ -986,6 +990,19 @@
         <v>15</v>
       </c>
       <c r="E18" s="5"/>
+    </row>
+    <row r="19" ht="15">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -1126,7 +1143,7 @@
     </row>
     <row r="9" ht="15">
       <c r="A9" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -1137,7 +1154,7 @@
     <row r="10" ht="15">
       <c r="A10" s="5"/>
       <c r="B10" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -1147,16 +1164,16 @@
     <row r="11" ht="15">
       <c r="A11" s="5"/>
       <c r="B11" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F11" s="5"/>
     </row>
@@ -1166,7 +1183,7 @@
         <v>19</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>15</v>
@@ -1180,7 +1197,7 @@
         <v>19</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>15</v>

</xml_diff>